<commit_message>
Update database files and Readme
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-types.xlsx
+++ b/backend/database/PostgreSQL-types.xlsx
@@ -4,19 +4,25 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="types" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>CREATE TYPE mod_tar AS ENUM ('convencional', 'verde', 'azul');</t>
+    <t>CREATE TYPE asset_type AS ENUM ('f', 'e', 'm', 't');</t>
+  </si>
+  <si>
+    <t>CREATE TYPE contract_item_type AS ENUM ('s', 'm');</t>
+  </si>
+  <si>
+    <t>CREATE TYPE modtar AS ENUM ('c', 'v', 'a');</t>
   </si>
 </sst>
 </file>
@@ -358,20 +364,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve some stuff in database
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-types.xlsx
+++ b/backend/database/PostgreSQL-types.xlsx
@@ -23,15 +23,9 @@
     <t>person_category_type</t>
   </si>
   <si>
-    <t>('F', 'E')</t>
-  </si>
-  <si>
     <t>('E', 'C', 'T', 'R')</t>
   </si>
   <si>
-    <t>facility, equipment</t>
-  </si>
-  <si>
     <t>efetivo, comissionado, terceirizado, estagiário</t>
   </si>
   <si>
@@ -60,6 +54,12 @@
   </si>
   <si>
     <t>elétrica, ar-condicionado, civil</t>
+  </si>
+  <si>
+    <t>('F', 'E', 'A')</t>
+  </si>
+  <si>
+    <t>facility, equipment, appliances</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,10 +419,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -430,43 +430,43 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +490,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>CONCATENATE("CREATE TYPE ",list!A1," AS ENUM ",list!B1,";")</f>
-        <v>CREATE TYPE asset_category_type AS ENUM ('F', 'E');</v>
+        <v>CREATE TYPE asset_category_type AS ENUM ('F', 'E', 'A');</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update orders table enums in db
</commit_message>
<xml_diff>
--- a/backend/database/PostgreSQL-types.xlsx
+++ b/backend/database/PostgreSQL-types.xlsx
@@ -38,28 +38,28 @@
     <t>order_category_type</t>
   </si>
   <si>
-    <t>('R', 'E', 'C', 'Z')</t>
-  </si>
-  <si>
-    <t>pendente de análise, em execução, concluída, cancelada</t>
-  </si>
-  <si>
-    <t>('H', 'N')</t>
-  </si>
-  <si>
-    <t>high, normal</t>
-  </si>
-  <si>
-    <t>('E', 'A', 'C')</t>
-  </si>
-  <si>
-    <t>elétrica, ar-condicionado, civil</t>
-  </si>
-  <si>
     <t>('F', 'E', 'A')</t>
   </si>
   <si>
     <t>facility, equipment, appliances</t>
+  </si>
+  <si>
+    <t>('CAN', 'NEG', 'PEN', 'SUS', 'FIL', 'EXE', 'CON')</t>
+  </si>
+  <si>
+    <t>cancelada, negada, pendente, suspenso, fila de espera, execução, concluída</t>
+  </si>
+  <si>
+    <t>('BAI', 'NOR', 'ALT', 'URG')</t>
+  </si>
+  <si>
+    <t>baixa, normal, alta, urgente</t>
+  </si>
+  <si>
+    <t>('EST', 'FOR', 'INF', 'ELE', 'HID', 'MAR', 'PIS', 'REV', 'VED', 'VID', 'SER')</t>
+  </si>
+  <si>
+    <t>avaliação estrutural, reparo em forro, infiltração, instalações elétricas, instalações hidrossanitárias, marcenaria, reparo em piso, revestimento, vedação espacial, vidraçaria/esquadria, serralheria</t>
   </si>
 </sst>
 </file>
@@ -95,8 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,14 +407,14 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -419,10 +422,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,7 +435,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -441,10 +444,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,21 +455,21 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -502,19 +505,19 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("CREATE TYPE ",list!A3," AS ENUM ",list!B3,";")</f>
-        <v>CREATE TYPE order_status_type AS ENUM ('R', 'E', 'C', 'Z');</v>
+        <v>CREATE TYPE order_status_type AS ENUM ('CAN', 'NEG', 'PEN', 'SUS', 'FIL', 'EXE', 'CON');</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE("CREATE TYPE ",list!A4," AS ENUM ",list!B4,";")</f>
-        <v>CREATE TYPE order_priority_type AS ENUM ('H', 'N');</v>
+        <v>CREATE TYPE order_priority_type AS ENUM ('BAI', 'NOR', 'ALT', 'URG');</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE("CREATE TYPE ",list!A5," AS ENUM ",list!B5,";")</f>
-        <v>CREATE TYPE order_category_type AS ENUM ('E', 'A', 'C');</v>
+        <v>CREATE TYPE order_category_type AS ENUM ('EST', 'FOR', 'INF', 'ELE', 'HID', 'MAR', 'PIS', 'REV', 'VED', 'VID', 'SER');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>